<commit_message>
Finished Stories and TPS Report
</commit_message>
<xml_diff>
--- a/Docs/TPS/TPS Report Fall 2019.xlsx
+++ b/Docs/TPS/TPS Report Fall 2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan_000\OneDrive - Western Michigan University\Senior Design Project 2019\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Western Michigan University\Megan N Solomon - Senior Design Project 2019\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="303" documentId="6_{AA6B608A-478B-44FB-A99C-A409A29ED0EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{B8A0B1A1-08FC-4A22-ACA8-C80E2E28498F}"/>
+  <xr:revisionPtr revIDLastSave="414" documentId="6_{AA6B608A-478B-44FB-A99C-A409A29ED0EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E018234D-CA91-45B4-A1D1-67A2DC705CCC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BC569457-A8D5-4039-9CF0-E7E82BD1501A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{BC569457-A8D5-4039-9CF0-E7E82BD1501A}"/>
   </bookViews>
   <sheets>
     <sheet name="TPS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="124">
   <si>
     <t>Task</t>
   </si>
@@ -176,9 +176,6 @@
     <t>5 hrs 30 mins</t>
   </si>
   <si>
-    <t>Had a meeting with larry on Thrusday to discuss progress on project</t>
-  </si>
-  <si>
     <t>45 mins</t>
   </si>
   <si>
@@ -242,18 +239,12 @@
     <t>Created a sprite that contains all the pizza slices for our game so it can load them all at once</t>
   </si>
   <si>
-    <t>Create spritesheet that has all 12 pieces to the pizza</t>
-  </si>
-  <si>
     <t>Get farmilier with Texture Packer for creating sprite sheets</t>
   </si>
   <si>
     <t>Create a layout for a game that follow the script for adding and subtraction factions</t>
   </si>
   <si>
-    <t>Start Development of Pizza Slicer</t>
-  </si>
-  <si>
     <t>Create game demo for larry to then display and show for grant money</t>
   </si>
   <si>
@@ -266,9 +257,6 @@
     <t>Create quiz for pizza slicer</t>
   </si>
   <si>
-    <t>Quiz Pop up for hints if the answer is wrong</t>
-  </si>
-  <si>
     <t>Resize the fractions and pizza slices</t>
   </si>
   <si>
@@ -348,6 +336,85 @@
   </si>
   <si>
     <t>Have meeting with database group to integrate game into their system as well as to test our scoring storage</t>
+  </si>
+  <si>
+    <t>Make more images such as, expert mode button, change the background for the title screen and game over screen, Change the take quiz button, and add a play again button</t>
+  </si>
+  <si>
+    <t>Have Megan's family test the game</t>
+  </si>
+  <si>
+    <t>They enjoyed the game but gave me a lot of feedback on what more we could do</t>
+  </si>
+  <si>
+    <t>Meet with Kapenga's son for some more suggestions for our game</t>
+  </si>
+  <si>
+    <t>Added a diffcult mode that takes away the slice visuals to force the user to added the fractions</t>
+  </si>
+  <si>
+    <t>Debug animation</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>6 Hr</t>
+  </si>
+  <si>
+    <t>animation was not working at all. Then finially got the animation to work. We discovered that the game was ending unexpectingly beucase it was check for gameover before it needed to</t>
+  </si>
+  <si>
+    <t>Not sure until further testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Showed Kapenga our game demo he gave us some feedback on changes that we should make to be user friendly
+</t>
+  </si>
+  <si>
+    <t>All buttons have been implemented and are functioning correctly</t>
+  </si>
+  <si>
+    <t>He gave us some great suggestions and we were able to replicate his design ideas and implement them successfully</t>
+  </si>
+  <si>
+    <t>Debug reset/play again button</t>
+  </si>
+  <si>
+    <t>We needed to make sure that the reset and play buttons take you back to the mode that you started in. The buttons need to be able to identify whether you started in normal mode or expert mode</t>
+  </si>
+  <si>
+    <t>Nick / Megan</t>
+  </si>
+  <si>
+    <t>Add the game to AWS</t>
+  </si>
+  <si>
+    <t>We did this so that anyone who would like to test or demo the game can access it from anywhere</t>
+  </si>
+  <si>
+    <t>Add dynamic hints to the game</t>
+  </si>
+  <si>
+    <t>Meet with the team</t>
+  </si>
+  <si>
+    <t>Hints now reflect the math that the student is actually attempting to solve</t>
+  </si>
+  <si>
+    <t>Our final meeting is complete. Our client and advisor are both satisfied with our project and we have a few things to finish up for them post graduation</t>
+  </si>
+  <si>
+    <t>Had a meeting with larry on Thursday to discuss progress on project</t>
+  </si>
+  <si>
+    <t>Create spritesheet that has all 12 pieces of the pizza</t>
+  </si>
+  <si>
+    <t>Start development of Pizza Slicer</t>
+  </si>
+  <si>
+    <t>Quiz pop up for hints if the answer is wrong</t>
   </si>
 </sst>
 </file>
@@ -506,8 +573,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7B7AEDDC-64B2-4088-8163-0F1DC74BDAFA}" name="Table2" displayName="Table2" ref="A2:I36" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A2:I36" xr:uid="{7AE42790-22BB-44AD-AADA-17522A5D9970}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7B7AEDDC-64B2-4088-8163-0F1DC74BDAFA}" name="Table2" displayName="Table2" ref="A2:I44" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A2:I44" xr:uid="{7AE42790-22BB-44AD-AADA-17522A5D9970}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D6C4E436-8634-4356-B857-E00D4995802B}" name="Task" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{2D11A8AB-02CD-42D0-B814-5A3B68D2CE27}" name="Who" dataDxfId="7"/>
@@ -823,26 +890,26 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="76" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>12</v>
       </c>
@@ -855,7 +922,7 @@
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -884,7 +951,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -913,7 +980,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -942,7 +1009,7 @@
         <v>43719</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -971,7 +1038,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1000,7 +1067,7 @@
         <v>43728</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1029,7 +1096,7 @@
         <v>43759</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1058,7 +1125,7 @@
         <v>43756</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1087,7 +1154,7 @@
         <v>43759</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
@@ -1116,9 +1183,9 @@
         <v>43745</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -1145,7 +1212,7 @@
         <v>43756</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -1165,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H12" s="2">
         <v>43738</v>
@@ -1174,7 +1241,7 @@
         <v>43759</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -1188,13 +1255,13 @@
         <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="2">
         <v>43738</v>
@@ -1203,9 +1270,9 @@
         <v>43759</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
@@ -1217,13 +1284,13 @@
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="2">
         <v>43745</v>
@@ -1232,9 +1299,9 @@
         <v>43748</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
@@ -1247,21 +1314,21 @@
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="2">
         <v>43752</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
@@ -1273,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="2">
         <v>43752</v>
@@ -1282,9 +1349,9 @@
         <v>43759</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>41</v>
@@ -1302,7 +1369,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H17" s="2">
         <v>43756</v>
@@ -1311,9 +1378,9 @@
         <v>43758</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>41</v>
@@ -1325,13 +1392,13 @@
         <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="H18" s="2">
         <v>43756</v>
@@ -1340,9 +1407,9 @@
         <v>43759</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>36</v>
@@ -1354,13 +1421,13 @@
         <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="2">
         <v>43756</v>
@@ -1369,15 +1436,15 @@
         <v>43758</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>33</v>
@@ -1389,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H20" s="2">
         <v>43756</v>
@@ -1398,12 +1465,12 @@
         <v>43758</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
@@ -1412,24 +1479,24 @@
         <v>33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F21" s="3">
         <v>0.8</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H21" s="2">
         <v>43756</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -1444,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H22" s="2">
         <v>43759</v>
@@ -1453,12 +1520,12 @@
         <v>43764</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
@@ -1473,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H23" s="2">
         <v>43759</v>
@@ -1482,9 +1549,9 @@
         <v>43764</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>41</v>
@@ -1496,13 +1563,13 @@
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F24" s="3">
         <v>1</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H24" s="2">
         <v>43766</v>
@@ -1511,9 +1578,9 @@
         <v>43766</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>41</v>
@@ -1531,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H25" s="2">
         <v>43766</v>
@@ -1540,9 +1607,9 @@
         <v>43766</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>41</v>
@@ -1560,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H26" s="2">
         <v>43766</v>
@@ -1569,27 +1636,27 @@
         <v>43771</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H27" s="2">
         <v>43766</v>
@@ -1598,9 +1665,9 @@
         <v>43771</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>9</v>
@@ -1618,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H28" s="2">
         <v>43766</v>
@@ -1627,9 +1694,9 @@
         <v>43769</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>36</v>
@@ -1647,7 +1714,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H29" s="2">
         <v>43773</v>
@@ -1656,9 +1723,9 @@
         <v>43776</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>41</v>
@@ -1676,7 +1743,7 @@
         <v>0.9</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H30" s="2">
         <v>43773</v>
@@ -1685,9 +1752,9 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>36</v>
@@ -1705,7 +1772,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H31" s="2">
         <v>43773</v>
@@ -1714,9 +1781,9 @@
         <v>43776</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>9</v>
@@ -1734,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H32" s="2">
         <v>43773</v>
@@ -1743,31 +1810,38 @@
         <v>43777</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="4"/>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="H33" s="2">
         <v>43780</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I33" s="2">
+        <v>43787</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>15</v>
@@ -1775,15 +1849,22 @@
       <c r="D34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="4"/>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="H34" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>41</v>
@@ -1800,23 +1881,265 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="H36" s="2">
         <v>43780</v>
+      </c>
+      <c r="I36" s="2">
+        <v>43786</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" s="2">
+        <v>43780</v>
+      </c>
+      <c r="I37" s="2">
+        <v>43786</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="74.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H38" s="2">
+        <v>43780</v>
+      </c>
+      <c r="I38" s="2">
+        <v>43787</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H39" s="2">
+        <v>43787</v>
+      </c>
+      <c r="I39" s="2">
+        <v>43790</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H40" s="2">
+        <v>43787</v>
+      </c>
+      <c r="I40" s="2">
+        <v>43790</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H41" s="2">
+        <v>43790</v>
+      </c>
+      <c r="I41" s="2">
+        <v>43791</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F42" s="3">
+        <v>1</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H42" s="2">
+        <v>43791</v>
+      </c>
+      <c r="I42" s="2">
+        <v>43793</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H43" s="2">
+        <v>43794</v>
+      </c>
+      <c r="I43" s="2">
+        <v>43808</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="3">
+        <v>1</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H44" s="2">
+        <v>43794</v>
+      </c>
+      <c r="I44" s="2">
+        <v>43810</v>
       </c>
     </row>
   </sheetData>
@@ -1832,12 +2155,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2012,15 +2332,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43D855AB-BBEE-4122-833D-D6FBA2A1E148}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D0E2AB9-B3EF-4FB9-8CB6-431A80FDAC33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2aed31c6-efa5-4803-9dcc-f21af739f51e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="70ff384a-49eb-425a-a776-6cfe091623e0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2045,18 +2377,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D0E2AB9-B3EF-4FB9-8CB6-431A80FDAC33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43D855AB-BBEE-4122-833D-D6FBA2A1E148}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2aed31c6-efa5-4803-9dcc-f21af739f51e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="70ff384a-49eb-425a-a776-6cfe091623e0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>